<commit_message>
user response is being passed properly
</commit_message>
<xml_diff>
--- a/Resources Version 3.xlsx
+++ b/Resources Version 3.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1611159482610805568</t>
+          <t>-5024543956076458118</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>-5000093523636905935</t>
+          <t>1089035699668342371</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>-9121236759796572734</t>
+          <t>-1244263580737547364</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>3578071969760317121</t>
+          <t>-161301453925448720</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>-1658038630144870832</t>
+          <t>6718241552717100685</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-8520959257517144337</t>
+          <t>-3905887755394201128</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>6208171667744997255</t>
+          <t>2087618240458196074</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>128276035495962274</t>
+          <t>-1133448472351489615</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>-8624872175284913876</t>
+          <t>-3754667236999779330</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-4996070703984182687</t>
+          <t>1437254590655497329</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2603356457869430791</t>
+          <t>-3904202706470053090</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>-2810285170997574971</t>
+          <t>3765829122322171259</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>-7295810977895708144</t>
+          <t>4443689924724281400</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>-5738464422319854763</t>
+          <t>342447401836312909</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>4498230918338648917</t>
+          <t>-3748958274366039936</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>-2024119470320247978</t>
+          <t>5373755885703083921</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1947718013068141847</t>
+          <t>234503726462468368</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>50636793026623891</t>
+          <t>2683659211737244996</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>5734418877753304704</t>
+          <t>2759954696691783152</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>8338627257222620405</t>
+          <t>-5187000563749245230</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>-8188834852230411745</t>
+          <t>1011090460398641051</t>
         </is>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>5831695281376826213</t>
+          <t>-4103418074422834420</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>7805668875972183313</t>
+          <t>-6376283724736182054</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>-3831684222430714367</t>
+          <t>5823057369151609802</t>
         </is>
       </c>
     </row>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>-492768234141851837</t>
+          <t>-5283959848959794851</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>-7464362164933313209</t>
+          <t>-7599315705937794156</t>
         </is>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>893734924921033968</t>
+          <t>-182851223443396917</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2323991885833396129</t>
+          <t>520941480054210267</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>5177575352705285819</t>
+          <t>8642926451828596316</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>-3885129668263864654</t>
+          <t>-7492451031478652905</t>
         </is>
       </c>
     </row>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>-6621108376802806299</t>
+          <t>1477741574240669269</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>-7441511921633054527</t>
+          <t>-7240450692410412136</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>-244818327928058060</t>
+          <t>6110845092117184315</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>662270420949487879</t>
+          <t>-967750167548269064</t>
         </is>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>-592181170195573142</t>
+          <t>-6575885249756271861</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>-3094326880485934967</t>
+          <t>5331645556016952874</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>1243852704491987656</t>
+          <t>-4262106502305468479</t>
         </is>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>4656235417474542947</t>
+          <t>-634420195667353983</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>942345159992927641</t>
+          <t>-2123348678845688084</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>-1331490742062606734</t>
+          <t>3044957725242547638</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>-35705589499922917</t>
+          <t>-1032778900891362717</t>
         </is>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>-3775303887887431374</t>
+          <t>9078632615318898839</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>-2373332318195140571</t>
+          <t>3721174555711123392</t>
         </is>
       </c>
     </row>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>7054354505219405091</t>
+          <t>-138546740687672117</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>-8695685075669419478</t>
+          <t>-4038202933620396616</t>
         </is>
       </c>
     </row>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>5986450936034174419</t>
+          <t>-7510076755748020832</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>7018813696181125731</t>
+          <t>400801814425465643</t>
         </is>
       </c>
     </row>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>-3361186204485173916</t>
+          <t>-5488338553918754255</t>
         </is>
       </c>
     </row>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>-5970164859841304846</t>
+          <t>-5894097881799099125</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>-225029014683973038</t>
+          <t>2674234454793678402</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>-9221795114204468306</t>
+          <t>-2770140877516060079</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>-7883903835120181722</t>
+          <t>6286707755240707741</t>
         </is>
       </c>
     </row>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>1644572709021230001</t>
+          <t>-8908226992892378639</t>
         </is>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>-9080935030185627671</t>
+          <t>-7477131404435700751</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>117401093753819157</t>
+          <t>338897088895821016</t>
         </is>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>5292114110727151300</t>
+          <t>-1126872237344345472</t>
         </is>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>-6868277026323875339</t>
+          <t>6862186950629248297</t>
         </is>
       </c>
     </row>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>-1525444627080313910</t>
+          <t>7036815626524267464</t>
         </is>
       </c>
     </row>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>6271369599070313965</t>
+          <t>-695862899884876166</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>1368437499332812569</t>
+          <t>-2587052032452335265</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>8526915679237418746</t>
+          <t>230596285226370772</t>
         </is>
       </c>
     </row>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>-1570667557615619297</t>
+          <t>-2541033976428744266</t>
         </is>
       </c>
     </row>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>-6382623478449572241</t>
+          <t>-1208576990337673422</t>
         </is>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>8724189165679688998</t>
+          <t>4368958120626670240</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>5225467105963592841</t>
+          <t>7720003327581256505</t>
         </is>
       </c>
     </row>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>5444755416007680024</t>
+          <t>-1887934018914723522</t>
         </is>
       </c>
     </row>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>-1985173836293427321</t>
+          <t>6952037141390866772</t>
         </is>
       </c>
     </row>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>-3713213461733172552</t>
+          <t>2155417342542719627</t>
         </is>
       </c>
     </row>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>-760881950853020343</t>
+          <t>6539586539588433881</t>
         </is>
       </c>
     </row>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>3741260800092316681</t>
+          <t>1994887170751869595</t>
         </is>
       </c>
     </row>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>5692554409426569150</t>
+          <t>4332347659672953139</t>
         </is>
       </c>
     </row>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>-3533873600700934908</t>
+          <t>-8399382642519882028</t>
         </is>
       </c>
     </row>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>-6813383974164297419</t>
+          <t>3965854485100243398</t>
         </is>
       </c>
     </row>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>-2286051782658980778</t>
+          <t>8208960443869166268</t>
         </is>
       </c>
     </row>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>-2600860881838309263</t>
+          <t>-353724325541503250</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>-7832515931302678321</t>
+          <t>-4987400653008156332</t>
         </is>
       </c>
     </row>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>270590289716822010</t>
+          <t>-5555794890157511271</t>
         </is>
       </c>
     </row>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>-2650486932505595026</t>
+          <t>-8628740675040476216</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>6869707514143123686</t>
+          <t>2879104050616670826</t>
         </is>
       </c>
     </row>
@@ -4753,7 +4753,7 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>-640863818679667677</t>
+          <t>7874896233432519209</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>-4315625748373867057</t>
+          <t>-8914059309599259301</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>-3981662387931563598</t>
+          <t>-6848150808824375545</t>
         </is>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>6391750645298659301</t>
+          <t>-8136266109847932246</t>
         </is>
       </c>
     </row>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>8241467780295571815</t>
+          <t>-802813319062420830</t>
         </is>
       </c>
     </row>
@@ -5015,7 +5015,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>5083716500831870541</t>
+          <t>-6736413499540721321</t>
         </is>
       </c>
     </row>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>-7368189064409504321</t>
+          <t>3917367986763808549</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>2661863771704923304</t>
+          <t>-379666681410107570</t>
         </is>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>-5096738911162879383</t>
+          <t>7882932941196884806</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>5419248776471514424</t>
+          <t>-7882385328087490693</t>
         </is>
       </c>
     </row>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>-3002906098690664285</t>
+          <t>4026045856970347435</t>
         </is>
       </c>
     </row>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>8126035522040270946</t>
+          <t>6023417813053480307</t>
         </is>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>-2161464074102322834</t>
+          <t>1454228011034335609</t>
         </is>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>-2422086215131871547</t>
+          <t>5025001820813646212</t>
         </is>
       </c>
     </row>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>-592411632281008049</t>
+          <t>6499918952172172178</t>
         </is>
       </c>
     </row>
@@ -5571,7 +5571,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>726507393764109245</t>
+          <t>9012395923092219144</t>
         </is>
       </c>
     </row>

</xml_diff>